<commit_message>
current version, team detail has been changed
</commit_message>
<xml_diff>
--- a/data/excel_inputs/input1.xlsx
+++ b/data/excel_inputs/input1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubCode\DCES Folder\LoLApiVersion1\data\excel_inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F590F25-6031-4694-8211-230B95AF29F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90ECED04-A173-4DBD-A416-10EA6064F4CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{452048D8-C31F-4CAC-8D67-32DE492E0EED}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -456,10 +456,10 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>7099400200</v>
@@ -487,10 +487,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -507,10 +507,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>

</xml_diff>